<commit_message>
Updated Recipes Excel file and SQL Database search method
</commit_message>
<xml_diff>
--- a/Database/RECIPES.xlsx
+++ b/Database/RECIPES.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\NetBeansProjects\PeasantKitchen\Database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12270" windowHeight="4080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Recipes" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Recipes" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Recipes</t>
   </si>
@@ -32,34 +39,22 @@
     <t>Spaghetti</t>
   </si>
   <si>
-    <t>2 Jars Pasta Sauce, 1 Box Spaghetti Noodles, 1 1/2 lb Ground Beef</t>
-  </si>
-  <si>
     <t>1. Boil Water, cook ground beef until brown 2. Drain grease from ground beef 3. Add noodles to water…cook until soft, add pasta sauce to ground beef and let simmer.</t>
   </si>
   <si>
     <t>Seasoned Chicken Wings</t>
   </si>
   <si>
-    <t>8 Chicken Wings, 1 Teaspoon of Olive Oil, 3 Tablespoons of butter, Seasoning, Ranch Dressing</t>
-  </si>
-  <si>
     <t>1. Heat Grill to Medium 2. Toss Wings with Olive Oil and Seasoning 3. Grill until cooked through, turn every 15 minutes 4. Mix seasoning/butter, toss with cooked wings and serve with ranch dressing.</t>
   </si>
   <si>
     <t>Teriyaki Wings</t>
   </si>
   <si>
-    <t>8 Chicken Wings, Teriyaki Sauce, Sesame Seeds</t>
-  </si>
-  <si>
     <t>1. Halve 8 chicken wings (about 1½ pounds) through the joint; cut off and discard the wing tips. Grill over medium-low heat, covered, turning occasionally, until cooked through, 20 to 25 minutes.                                                             2.Brush with ¼ cup teriyaki sauce during the last 5 minutes of grilling. Sprinkle with ½ teaspoon toasted sesame seeds and serve with additional teriyaki sauce for dipping, if desired.</t>
   </si>
   <si>
     <t>Chicken with Lemons and Olives</t>
-  </si>
-  <si>
-    <t>2 1/2 - 3 lbs Chicken w Bone, Salt, Pepper, 2 teaspoons olive oil, 1 Lemon, 1/2 cup pitted olives</t>
   </si>
   <si>
     <t>1. Heat oven to 400° F. Season the chicken with ½ teaspoon salt and ¼ teaspoon pepper.
@@ -70,25 +65,16 @@
     <t>Cheese Quesadilla</t>
   </si>
   <si>
-    <t>2 Flour Tortillas, Shredded Cheese</t>
-  </si>
-  <si>
     <t>1. Spread shredded cheese over tortilla on frying pan                                                          2. Place other tortilla on top                                   3. Cook until lightly melted                                    4. Flip Quesadilla, Cook until Fully Meted</t>
   </si>
   <si>
     <t>Chicken Quesadilla</t>
   </si>
   <si>
-    <t xml:space="preserve">2 Flour Tortillas, Shredded Cheese, 1 Boneless Chicken Breast </t>
-  </si>
-  <si>
     <t>1. Chop Chicken Breast into small pieces                2. Cook Chicken Pieces fully                                 3. Spread shredded cheese over tortilla on frying pan                                                          4. Mix in chicken pieces and place other tortilla on top                                                                 5. Cook until lightly melted                                    6. Flip Quesadilla, Cook until Fully Meted</t>
   </si>
   <si>
     <t>Beef Kabobs w Lime</t>
-  </si>
-  <si>
-    <t>1/4 Medium Watermelon, 1/4 Red Onion, Salt, Pepper, 1 1/2 lbs tri tip, 8 red peppers, 1 lime</t>
   </si>
   <si>
     <t>1. Heat grill to medium-high. Soak 8 wooden skewers for 10 minutes.
@@ -100,18 +86,12 @@
     <t>Quick and Easy Lasagna</t>
   </si>
   <si>
-    <t>26 ounce Jar Pasta Sauce, Bag of Frozen Ravioli, Chopped Spinach, Shredded Mozzarella, Grated Parmesan Cheese</t>
-  </si>
-  <si>
     <t>1. Heat oven to 350° F. Coat a 13-by-9-inch baking dish with cooking spray and spoon in a third of the sauce.
 2. Arrange 12 ravioli on top and scatter the spinach over them. Top with half of each cheese. Cover with another layer of ravioli and the remaining sauce and cheese.
 3. Cover with foil and bake 25 minutes. Uncover and bake 5 to 10 minutes more or until bubbly.</t>
   </si>
   <si>
     <t>Mac n Cheese</t>
-  </si>
-  <si>
-    <t>5 Tablespoons of Butter, 1 lb of Macaroni Noodles, 1/2 cup of flour, 6 cups of whole milk, 2 cups of Grated Gruyere, 1 1/2 cups of Grated Cheddar, 1/4 teaspoons of Cayenne Pepper, Salt</t>
   </si>
   <si>
     <t>1. Heat oven to 400° F. Butter a 9-by-13-inch baking dish or some other shallow 3-quart baking dish.
@@ -123,22 +103,49 @@
     <t>Easy Tacos</t>
   </si>
   <si>
-    <t>1 lb ground beef, Salsa, 10 Taco Shells, 1/2 head shredded lettuce, 1 medium chopped tomato, 1 cup shredded cheese</t>
-  </si>
-  <si>
     <t>1. Cook beef in 10-inch skillet over medium heat 8 to 10 minutes, stirring occasionally, until brown; drain.
 2. Stir salsa into beef. Heat to boiling, stirring constantly; reduce heat to medium-low. Cook 5 minutes, stirring occasionally. Pour beef mixture into large serving bowl.
 3. Heat taco shells as directed on package. Serve taco shells with beef mixture, lettuce, tomato and cheese.</t>
+  </si>
+  <si>
+    <t>&lt;24&gt;&lt;Ounces&gt;&lt;Pasta Sauce&gt;,&lt;1&gt;&lt;Box&gt;&lt;Spaghetti Noodles&gt;,&lt;1.5&gt;&lt;lb&gt;&lt;Ground Beef&gt;</t>
+  </si>
+  <si>
+    <t>&lt;8&gt;&lt;&gt;&lt;Chicken Wings&gt;, &lt;1&gt;&lt;Teaspoon&gt; &lt;Olive Oil&gt;,&lt;3&gt;&lt;Tablespoons&gt;&lt;butter&gt;,&lt;&gt;&lt;&gt;&lt;Seasoning&gt;</t>
+  </si>
+  <si>
+    <t>&lt;8&gt;&lt;&gt;&lt;Chicken Wings&gt;,&lt;&gt;&lt;&gt;&lt;Teriyaki Sauce&gt;,&lt;&gt;&lt;&gt;&lt;Sesame Seeds&gt;</t>
+  </si>
+  <si>
+    <t>&lt;2.5 - 3&gt;&lt;lbs&gt;&lt;Chicken with Bone&gt;,&lt;&gt;&lt;&gt;&lt;Salt&gt;,&lt;&gt;&lt;&gt;&lt;Pepper&gt;,&lt;2&gt;&lt;teaspoons&gt;&lt;olive oil&gt;,&lt;1&gt;&lt;&gt;&lt;Lemon&gt;, &lt;.5&gt;&lt;cup&gt;&lt;pitted olives&gt;</t>
+  </si>
+  <si>
+    <t>&lt;2&gt;&lt;&gt;&lt;Flour Tortillas&gt;,&lt;&gt;&lt;&gt;&lt;Shredded Cheese&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;2&gt;&lt;&gt;&lt;Flour Tortillas&gt;,&lt;&gt;&lt;&gt;&lt;Shredded Cheese&gt;,&lt;1&gt;&lt;&gt;&lt;Boneless Chicken Breast&gt;  </t>
+  </si>
+  <si>
+    <t>&lt;.25&gt;&lt;&gt;&lt;Medium Watermelon&gt;,&lt;.25&gt;&lt;&gt;&lt;Red Onion&gt;,&lt;&gt;&lt;&gt;&lt;Salt&gt;,&lt;&gt;&lt;&gt;&lt;Pepper&gt;,&lt;1.5&gt;&lt;lbs&gt;&lt;tri tip&gt;,&lt;8&gt;&lt;&gt;&lt;red peppers&gt;,&lt;1&gt;&lt;&gt;&lt;lime&gt;</t>
+  </si>
+  <si>
+    <t>&lt;26&gt;&lt;ounce Jar&gt;&lt;Pasta Sauce&gt;,&lt;1&gt;&lt;Bag&gt;&lt;Frozen Ravioli&gt;,&lt;&gt;&lt;&gt;&lt;Chopped Spinach&gt;,&lt;&gt;&lt;&gt;&lt;Shredded Mozzarella&gt;,&lt;&gt;&lt;&gt;&lt;Grated Parmesan Cheese&gt;</t>
+  </si>
+  <si>
+    <t>&lt;5&gt;&lt;Tablespoons&gt;&lt;Butter&gt;,&lt;1&gt;&lt;lb&gt;&lt;Macaroni Noodles&gt;,&lt;.5&gt;&lt;cup&gt;&lt;flour&gt;,&lt;6&gt;&lt;cups&gt;&lt;whole milk&gt;,&lt;2&gt;&lt;cups&gt;&lt;Grated Gruyere&gt;,&lt;1.5&gt;&lt;cups&gt;&lt;Grated Cheddar&gt;,&lt;.25&gt;&lt;teaspoons&gt;&lt;Cayenne Pepper&gt;,&lt;&gt;&lt;&gt;&lt;Salt&gt;</t>
+  </si>
+  <si>
+    <t>&lt;1&gt;&lt;lb&gt;&lt;ground beef&gt;,&lt;&gt;&lt;&gt;&lt;Salsa&gt;,&lt;10&gt;&lt;&gt;&lt;Taco Shells&gt;,&lt;.5&gt;&lt;head&gt;&lt;shredded lettuce&gt;,&lt;1&gt;&lt;&gt;&lt;medium chopped tomato&gt;,&lt;1&gt;&lt;cup&gt;&lt;shredded cheese&gt;</t>
+  </si>
+  <si>
+    <t>NUM_INGR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -150,7 +157,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -291,49 +298,49 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -343,26 +350,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -488,7 +554,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -497,7 +563,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -506,7 +572,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -570,8 +636,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -579,7 +645,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -587,7 +653,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -606,7 +672,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -614,7 +680,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -642,7 +708,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -668,7 +734,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -694,7 +760,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -720,7 +786,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -746,7 +812,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -772,7 +838,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -798,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -824,7 +890,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -850,7 +916,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -863,9 +929,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -882,7 +954,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -901,7 +973,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,7 +999,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +1025,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1051,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1077,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,7 +1103,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1057,7 +1129,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1083,7 +1155,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1109,7 +1181,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1135,7 +1207,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1148,9 +1220,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1164,7 +1242,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1183,7 +1261,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1213,7 +1291,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1239,7 +1317,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1343,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,7 +1369,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1395,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,7 +1421,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1369,7 +1447,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1395,7 +1473,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1421,7 +1499,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1434,294 +1512,328 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E23"/>
+  <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1797" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.6016" style="1" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="1" customWidth="1"/>
+    <col min="6" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" ht="56.55" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6">
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="56.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" ht="68.35" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9">
+      <c r="D4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="116.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1">
         <v>2</v>
       </c>
-      <c r="C4" t="s" s="10">
+    </row>
+    <row r="8" spans="1:6" ht="104.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="128.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="10">
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="200.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8">
         <v>9</v>
       </c>
-      <c r="E4" t="s" s="10">
+      <c r="C11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="128.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" ht="116.35" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s" s="10">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" ht="140.35" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" ht="68.35" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s" s="10">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" ht="104.35" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9">
+      <c r="C12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1">
         <v>6</v>
       </c>
-      <c r="C8" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s" s="10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" ht="140.35" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s" s="10">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s" s="10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" ht="128.35" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="10">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" ht="200.35" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s" s="10">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s" s="10">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" ht="128.35" customHeight="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s" s="10">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>